<commit_message>
checkpoint: some of the runs of NQueens, and all the variants of TSP
</commit_message>
<xml_diff>
--- a/MetaheuristicOptimization/Assignment2/Book1.xlsx
+++ b/MetaheuristicOptimization/Assignment2/Book1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbhatta1\dev\ml-assignments\MetaheuristicOptimization\Assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{352B3496-FB76-4D41-9EDF-64204504B45B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CF7FD4-7862-4F2D-AE57-DF690F62D8F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-120" windowWidth="28080" windowHeight="16440"/>
+    <workbookView xWindow="840" yWindow="-120" windowWidth="28080" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
   <si>
     <t>Run 1</t>
   </si>
@@ -66,13 +68,46 @@
   </si>
   <si>
     <t>getHeuristicCost</t>
+  </si>
+  <si>
+    <t>restart_and_iterate</t>
+  </si>
+  <si>
+    <t>restart_and_iterate with cache</t>
+  </si>
+  <si>
+    <t>get_distance</t>
+  </si>
+  <si>
+    <t>get_distance with cache</t>
+  </si>
+  <si>
+    <t>is_valid_swap</t>
+  </si>
+  <si>
+    <t>Calls</t>
+  </si>
+  <si>
+    <t>is_valid_swap with cache</t>
+  </si>
+  <si>
+    <t>Improvement (%)</t>
+  </si>
+  <si>
+    <t>12544  calls</t>
+  </si>
+  <si>
+    <t>671104 calls</t>
+  </si>
+  <si>
+    <t>Improvement from Base (%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,8 +115,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,6 +143,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -113,10 +162,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,16 +481,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
@@ -449,34 +501,36 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C4">
@@ -505,7 +559,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C5">
@@ -534,7 +588,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C6">
@@ -563,67 +617,69 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2">
-        <f>AVERAGE(C4:C6)</f>
+      <c r="C7" s="1">
+        <f t="shared" ref="C7:I7" si="0">AVERAGE(C4:C6)</f>
         <v>32.203333333333333</v>
       </c>
-      <c r="D7" s="2">
-        <f>AVERAGE(D4:D6)</f>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
         <v>23.26</v>
       </c>
-      <c r="E7" s="2">
-        <f>AVERAGE(E4:E6)</f>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
         <v>27.671212260262426</v>
       </c>
-      <c r="F7" s="2">
-        <f>AVERAGE(F4:F6)</f>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
         <v>11.673333333333332</v>
       </c>
-      <c r="G7" s="2">
-        <f>AVERAGE(G4:G6)</f>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
         <v>63.703083441476984</v>
       </c>
-      <c r="H7" s="2">
-        <f>AVERAGE(H4:H6)</f>
+      <c r="H7" s="1">
+        <f t="shared" si="0"/>
         <v>7.330000000000001</v>
       </c>
-      <c r="I7" s="2">
-        <f>AVERAGE(I4:I6)</f>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
         <v>77.206421078918595</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C10">
@@ -652,7 +708,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C11">
@@ -681,7 +737,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C12">
@@ -710,39 +766,468 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="2">
-        <f>AVERAGE(C10:C12)</f>
+      <c r="C13" s="1">
+        <f t="shared" ref="C13:I13" si="1">AVERAGE(C10:C12)</f>
         <v>7.9766666666666675</v>
       </c>
-      <c r="D13" s="2">
-        <f>AVERAGE(D10:D12)</f>
+      <c r="D13" s="1">
+        <f t="shared" si="1"/>
         <v>5.6833333333333336</v>
       </c>
-      <c r="E13" s="2">
-        <f>AVERAGE(E10:E12)</f>
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
         <v>28.67582339095668</v>
       </c>
-      <c r="F13" s="2">
-        <f>AVERAGE(F10:F12)</f>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
         <v>3.0333333333333332</v>
       </c>
-      <c r="G13" s="2">
-        <f>AVERAGE(G10:G12)</f>
+      <c r="G13" s="1">
+        <f t="shared" si="1"/>
         <v>61.933776892326954</v>
       </c>
-      <c r="H13" s="2">
-        <f>AVERAGE(H10:H12)</f>
+      <c r="H13" s="1">
+        <f t="shared" si="1"/>
         <v>1.33</v>
       </c>
-      <c r="I13" s="2">
-        <f>AVERAGE(I10:I12)</f>
+      <c r="I13" s="1">
+        <f t="shared" si="1"/>
         <v>83.299686349507553</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06458EC0-38A4-4D03-812C-BF2A15BF63E1}">
+  <dimension ref="B6:G18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>33.79</v>
+      </c>
+      <c r="E7">
+        <v>23.27</v>
+      </c>
+      <c r="F7">
+        <v>11.63</v>
+      </c>
+      <c r="G7">
+        <v>7.32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>31.96</v>
+      </c>
+      <c r="E8">
+        <v>23.25</v>
+      </c>
+      <c r="F8">
+        <v>11.85</v>
+      </c>
+      <c r="G8">
+        <v>7.35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>30.86</v>
+      </c>
+      <c r="E9">
+        <v>23.26</v>
+      </c>
+      <c r="F9">
+        <v>11.54</v>
+      </c>
+      <c r="G9">
+        <v>7.32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" ref="D10:G10" si="0">AVERAGE(D7:D9)</f>
+        <v>32.203333333333333</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>23.26</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>11.673333333333332</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
+        <v>7.330000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="3">
+        <f>(D10-E10)/D10*100</f>
+        <v>27.771452230617943</v>
+      </c>
+      <c r="F11" s="3">
+        <f>(D10-F10)/D10*100</f>
+        <v>63.751164475727151</v>
+      </c>
+      <c r="G11" s="3">
+        <f>(D10-G10)/D10*100</f>
+        <v>77.238381119966874</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>8.32</v>
+      </c>
+      <c r="E14">
+        <v>5.69</v>
+      </c>
+      <c r="F14">
+        <v>3.02</v>
+      </c>
+      <c r="G14">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>7.92</v>
+      </c>
+      <c r="E15">
+        <v>5.67</v>
+      </c>
+      <c r="F15">
+        <v>3.08</v>
+      </c>
+      <c r="G15">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>7.69</v>
+      </c>
+      <c r="E16">
+        <v>5.69</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" ref="D17:G17" si="1">AVERAGE(D14:D16)</f>
+        <v>7.9766666666666675</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="1"/>
+        <v>5.6833333333333336</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="1"/>
+        <v>3.0333333333333332</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="1"/>
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="3">
+        <f>(D17-E17)/D17*100</f>
+        <v>28.750522356874221</v>
+      </c>
+      <c r="F18" s="3">
+        <f>(D17-F17)/D17*100</f>
+        <v>61.972419557041377</v>
+      </c>
+      <c r="G18" s="3">
+        <f>(D17-G17)/D17*100</f>
+        <v>83.326368575010449</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{910577BA-5226-465C-A0C6-1B7D766C47FB}">
+  <dimension ref="B3:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="B3:H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>6004640</v>
+      </c>
+      <c r="F4">
+        <v>6004640</v>
+      </c>
+      <c r="G4">
+        <v>1498770</v>
+      </c>
+      <c r="H4">
+        <v>1498770</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>12.39</v>
+      </c>
+      <c r="D5">
+        <v>5.35</v>
+      </c>
+      <c r="E5">
+        <v>5.4</v>
+      </c>
+      <c r="F5">
+        <v>7.1830000000000005E-2</v>
+      </c>
+      <c r="G5">
+        <v>1.94</v>
+      </c>
+      <c r="H5">
+        <v>4.4699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>14.63</v>
+      </c>
+      <c r="D6">
+        <v>5.66</v>
+      </c>
+      <c r="E6">
+        <v>6.09</v>
+      </c>
+      <c r="F6">
+        <v>7.9969999999999999E-2</v>
+      </c>
+      <c r="G6">
+        <v>1.5</v>
+      </c>
+      <c r="H6">
+        <v>4.8309999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>14.03</v>
+      </c>
+      <c r="D7">
+        <v>5.69</v>
+      </c>
+      <c r="E7">
+        <v>5.98</v>
+      </c>
+      <c r="F7">
+        <v>8.2890000000000005E-2</v>
+      </c>
+      <c r="G7">
+        <v>2.19</v>
+      </c>
+      <c r="H7">
+        <v>5.2130000000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <f>AVERAGE(C5:C7)</f>
+        <v>13.683333333333335</v>
+      </c>
+      <c r="D8">
+        <f>AVERAGE(D5:D7)</f>
+        <v>5.5666666666666664</v>
+      </c>
+      <c r="E8">
+        <f>AVERAGE(E5:E7)</f>
+        <v>5.8233333333333333</v>
+      </c>
+      <c r="F8">
+        <f>AVERAGE(F5:F7)</f>
+        <v>7.8230000000000008E-2</v>
+      </c>
+      <c r="G8">
+        <f>AVERAGE(G5:G7)</f>
+        <v>1.8766666666666667</v>
+      </c>
+      <c r="H8">
+        <f>AVERAGE(H5:H7)</f>
+        <v>4.8379999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1">
+        <f>(C8-D8)/C8*100</f>
+        <v>59.317904993909877</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1">
+        <f>(E8-F8)/E8*100</f>
+        <v>98.656611333714949</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1">
+        <f>(G8-H8)/G8*100</f>
+        <v>97.42202486678508</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>